<commit_message>
added basic xml creation
</commit_message>
<xml_diff>
--- a/assets/template-general.xlsx
+++ b/assets/template-general.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FabianBendun\Documents\Coding\round-table\finance-app\club-finances\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B040F5D4-BF03-41C5-8D87-B2714BE18F54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C306FDBC-0181-4D88-8D01-B532560AF393}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28695" yWindow="0" windowWidth="29010" windowHeight="15585" xr2:uid="{21810A49-7A37-48BB-AFF7-A95252713074}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{21810A49-7A37-48BB-AFF7-A95252713074}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>id</t>
   </si>
@@ -50,7 +50,28 @@
     <t>Ausfallbeitrag</t>
   </si>
   <si>
-    <t>Clubnummer</t>
+    <t>recipient</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>iban</t>
+  </si>
+  <si>
+    <t>bic</t>
+  </si>
+  <si>
+    <t>DE1234</t>
+  </si>
+  <si>
+    <t>MLPDEBXX</t>
+  </si>
+  <si>
+    <t>mandate</t>
+  </si>
+  <si>
+    <t>ABCDEF</t>
   </si>
 </sst>
 </file>
@@ -411,44 +432,61 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F0E028D-D745-45E9-9202-F7C97B097352}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
         <v>9</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
+      <c r="G2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>